<commit_message>
Bug Fixed (Some products without price, empty url)
</commit_message>
<xml_diff>
--- a/data/setting.xlsx
+++ b/data/setting.xlsx
@@ -451,21 +451,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>aaaa</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>aaaa</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>